<commit_message>
Finish chain from csv to a hashtable of perform categories
</commit_message>
<xml_diff>
--- a/Assets/Data/skill_categories.xlsx
+++ b/Assets/Data/skill_categories.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2180" yWindow="2540" windowWidth="25600" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="skill_categories.csv" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>name</t>
   </si>
@@ -51,9 +51,6 @@
     <t>scope</t>
   </si>
   <si>
-    <t>single</t>
-  </si>
-  <si>
     <t>shoot</t>
   </si>
   <si>
@@ -67,6 +64,9 @@
   </si>
   <si>
     <t>#id</t>
+  </si>
+  <si>
+    <t>impact coords</t>
   </si>
 </sst>
 </file>
@@ -115,8 +115,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -127,13 +129,15 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -463,22 +467,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -496,16 +503,19 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>1</v>
       </c>
@@ -518,16 +528,19 @@
       <c r="E2">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
-        <v>10</v>
+      <c r="H2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
@@ -535,36 +548,39 @@
       <c r="E3">
         <v>5</v>
       </c>
-      <c r="G3" t="s">
-        <v>10</v>
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4">
         <v>5</v>
       </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4">
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
@@ -572,10 +588,10 @@
       <c r="E5">
         <v>6</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>9</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finish convert relative coords to absolute coords
</commit_message>
<xml_diff>
--- a/Assets/Data/skill_categories.xlsx
+++ b/Assets/Data/skill_categories.xlsx
@@ -54,9 +54,6 @@
     <t>shoot</t>
   </si>
   <si>
-    <t>arrow</t>
-  </si>
-  <si>
     <t>line</t>
   </si>
   <si>
@@ -67,6 +64,9 @@
   </si>
   <si>
     <t>impact coords</t>
+  </si>
+  <si>
+    <t>penetrate</t>
   </si>
 </sst>
 </file>
@@ -470,7 +470,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -485,7 +485,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -503,7 +503,7 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
@@ -540,7 +540,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
@@ -560,16 +560,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4">
         <v>5</v>
       </c>
       <c r="H4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I4">
         <v>5</v>
@@ -580,7 +580,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>

</xml_diff>